<commit_message>
update Grobkonzept4.tex  text & inhalt tabelle
Eintrittwahschreinlichkeit/schaden->risiko grafik.xlsx
</commit_message>
<xml_diff>
--- a/PflichtenheftOrg/Ext. files/risiko grafik.xlsx
+++ b/PflichtenheftOrg/Ext. files/risiko grafik.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ramiro18/Library/Group Containers/UBF8T346G9.ms/MerpTempItems/Schule/Studium/Pro1/PflichtenheftOrg/Ext. files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D01B230D-AE05-9442-AD59-2CB8FB1B1C81}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B495E18-F7ED-174D-ACF1-291F8F004929}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{61394468-9DFD-4F2A-BFA1-329580A626FA}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="16180" xr2:uid="{61394468-9DFD-4F2A-BFA1-329580A626FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>Gross</t>
   </si>
@@ -60,12 +60,6 @@
     <t>Buget-überschreitung &gt;25%</t>
   </si>
   <si>
-    <t>Verzug &lt;10%</t>
-  </si>
-  <si>
-    <t>Verzug &gt;25%</t>
-  </si>
-  <si>
     <t>Buget-überschreitung 10% - 25%</t>
   </si>
   <si>
@@ -79,6 +73,39 @@
   </si>
   <si>
     <t>Verzug         10% - 25%</t>
+  </si>
+  <si>
+    <t>Eintritt   des Risiko</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
+  </si>
+  <si>
+    <t>Gering              1</t>
+  </si>
+  <si>
+    <t>Mässig               2</t>
+  </si>
+  <si>
+    <t>Hoch                3</t>
+  </si>
+  <si>
+    <t>Kaum         &lt;30%</t>
+  </si>
+  <si>
+    <t>Halb-halb          30-70%</t>
+  </si>
+  <si>
+    <t>(fast) sicher          &gt;70%</t>
+  </si>
+  <si>
+    <t>Auswirkung/Schaden</t>
+  </si>
+  <si>
+    <t>Verzug             &lt;10%</t>
+  </si>
+  <si>
+    <t>Verzug                &gt;25%</t>
   </si>
 </sst>
 </file>
@@ -371,7 +398,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -408,16 +435,30 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -427,23 +468,21 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -764,10 +803,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CDAB4DB-A61E-4AD2-A0F5-F92813AE6B2A}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -790,8 +829,8 @@
     </row>
     <row r="2" spans="1:7" ht="100" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
-      <c r="B2" s="15" t="s">
-        <v>4</v>
+      <c r="B2" s="21" t="s">
+        <v>23</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>0</v>
@@ -809,14 +848,14 @@
     </row>
     <row r="3" spans="1:7" ht="100" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
-      <c r="B3" s="15"/>
+      <c r="B3" s="21"/>
       <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="8">
         <v>2</v>
       </c>
-      <c r="E3" s="16">
+      <c r="E3" s="14">
         <v>4</v>
       </c>
       <c r="F3" s="4">
@@ -826,7 +865,7 @@
     </row>
     <row r="4" spans="1:7" ht="100" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13"/>
-      <c r="B4" s="15"/>
+      <c r="B4" s="21"/>
       <c r="C4" s="5" t="s">
         <v>2</v>
       </c>
@@ -859,11 +898,11 @@
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
       <c r="C6" s="12"/>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
       <c r="G6" s="13"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -887,61 +926,182 @@
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F9" s="13"/>
     </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+    </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C14" s="17"/>
-      <c r="D14" s="18" t="s">
+      <c r="A14" s="13"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="19"/>
-      <c r="F14" s="20"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="13"/>
     </row>
     <row r="15" spans="1:7" ht="34" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="23" t="s">
+      <c r="A15" s="13"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="25" t="s">
+      <c r="D15" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="26" t="s">
+      <c r="G15" s="13"/>
+    </row>
+    <row r="16" spans="1:7" ht="56.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="13"/>
+    </row>
+    <row r="17" spans="1:7" ht="56.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="13"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="24" t="s">
+      <c r="F17" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="13"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="13"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="23"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="13"/>
+    </row>
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="13"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" s="13"/>
+    </row>
+    <row r="23" spans="1:7" ht="32" x14ac:dyDescent="0.25">
+      <c r="A23" s="13"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="25" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="56.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" s="22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="3:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="F17" s="21" t="s">
-        <v>11</v>
-      </c>
+      <c r="D23" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="G23" s="13"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="13"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="13"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="D6:F6"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D21:F21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>